<commit_message>
Minor bugfixes that made it run on both datasets
</commit_message>
<xml_diff>
--- a/DD_Project/data/Niedermayer/statistical_tests/statistical_tests_results.xlsx
+++ b/DD_Project/data/Niedermayer/statistical_tests/statistical_tests_results.xlsx
@@ -530,10 +530,10 @@
         <v>2.611035721775769</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0985118738462704</v>
+        <v>0.1005870299094374</v>
       </c>
       <c r="I2" t="n">
-        <v>1.652111250732616</v>
+        <v>1.642014351456121</v>
       </c>
     </row>
     <row r="3">
@@ -557,10 +557,10 @@
         <v>-1.886925991587385</v>
       </c>
       <c r="H3" t="n">
-        <v>1.025217661732381e-45</v>
+        <v>5.14172098898158e-42</v>
       </c>
       <c r="I3" t="n">
-        <v>-14.19211342897858</v>
+        <v>-13.58170251854409</v>
       </c>
     </row>
     <row r="4">
@@ -584,10 +584,10 @@
         <v>7.18280400982161</v>
       </c>
       <c r="H4" t="n">
-        <v>2.453444895432948e-79</v>
+        <v>2.46192811623977e-69</v>
       </c>
       <c r="I4" t="n">
-        <v>18.85954013108411</v>
+        <v>17.60003022547899</v>
       </c>
     </row>
     <row r="5">
@@ -611,10 +611,10 @@
         <v>4.604144728265748</v>
       </c>
       <c r="H5" t="n">
-        <v>6.212148265041381e-18</v>
+        <v>9.753236417151387e-18</v>
       </c>
       <c r="I5" t="n">
-        <v>8.628574219881331</v>
+        <v>8.576819651182786</v>
       </c>
     </row>
     <row r="6">
@@ -638,10 +638,10 @@
         <v>4.836262268888744</v>
       </c>
       <c r="H6" t="n">
-        <v>1.486122013157329e-23</v>
+        <v>1.070470095212138e-23</v>
       </c>
       <c r="I6" t="n">
-        <v>10.00249017767423</v>
+        <v>10.03491920089278</v>
       </c>
     </row>
     <row r="7">
@@ -669,10 +669,10 @@
         <v>2.911860544057738</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0006285014647637549</v>
+        <v>0.001396946837793676</v>
       </c>
       <c r="I7" t="n">
-        <v>3.41900684024007</v>
+        <v>3.195281150425419</v>
       </c>
     </row>
     <row r="8">
@@ -696,10 +696,10 @@
         <v>18.26489919888875</v>
       </c>
       <c r="H8" t="n">
-        <v>5.221682299548872e-143</v>
+        <v>7.983756059632076e-196</v>
       </c>
       <c r="I8" t="n">
-        <v>25.46182791351096</v>
+        <v>29.85317630367946</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         <v>-13.95094143674026</v>
       </c>
       <c r="H9" t="n">
-        <v>1.824851313479425e-134</v>
+        <v>7.793518645540226e-99</v>
       </c>
       <c r="I9" t="n">
-        <v>-24.67839335173875</v>
+        <v>-21.10096151109139</v>
       </c>
     </row>
     <row r="10">
@@ -744,16 +744,16 @@
         <v>-8.597604571087324</v>
       </c>
       <c r="F10" t="n">
-        <v>4.090125119497237e-14</v>
+        <v>4.090125119497236e-14</v>
       </c>
       <c r="G10" t="n">
         <v>-8.819416807040355</v>
       </c>
       <c r="H10" t="n">
-        <v>5.206155859702213e-43</v>
+        <v>1.626712725324637e-42</v>
       </c>
       <c r="I10" t="n">
-        <v>-13.74840939866565</v>
+        <v>-13.66572687144085</v>
       </c>
     </row>
     <row r="11">
@@ -777,10 +777,10 @@
         <v>-10.02712355821534</v>
       </c>
       <c r="H11" t="n">
-        <v>1.078759060277649e-44</v>
+        <v>3.762217274443967e-48</v>
       </c>
       <c r="I11" t="n">
-        <v>-14.02613269218619</v>
+        <v>-14.58005350840661</v>
       </c>
     </row>
     <row r="12">
@@ -808,10 +808,10 @@
         <v>6.219060602798643</v>
       </c>
       <c r="H12" t="n">
-        <v>1.076789334270925e-20</v>
+        <v>1.283794319129071e-21</v>
       </c>
       <c r="I12" t="n">
-        <v>9.328205053014493</v>
+        <v>9.551057208083092</v>
       </c>
     </row>
     <row r="13">
@@ -835,10 +835,10 @@
         <v>21.49354292899049</v>
       </c>
       <c r="H13" t="n">
-        <v>1.5083046905637e-275</v>
+        <v>1.349055976310105e-250</v>
       </c>
       <c r="I13" t="n">
-        <v>35.46842783786452</v>
+        <v>33.81122331986262</v>
       </c>
     </row>
     <row r="14">
@@ -862,10 +862,10 @@
         <v>-12.99353752381963</v>
       </c>
       <c r="H14" t="n">
-        <v>3.885738258551029e-93</v>
+        <v>1.070148427334821e-102</v>
       </c>
       <c r="I14" t="n">
-        <v>-20.47124402550113</v>
+        <v>-21.51739207891101</v>
       </c>
     </row>
     <row r="15">
@@ -889,10 +889,10 @@
         <v>-8.073719604570949</v>
       </c>
       <c r="H15" t="n">
-        <v>3.888864808655911e-40</v>
+        <v>1.740138330085494e-36</v>
       </c>
       <c r="I15" t="n">
-        <v>-13.26114992207716</v>
+        <v>-12.6152458157533</v>
       </c>
     </row>
     <row r="16">
@@ -916,10 +916,10 @@
         <v>-6.455361578813921</v>
       </c>
       <c r="H16" t="n">
-        <v>4.614493385697617e-30</v>
+        <v>1.0665277478531e-29</v>
       </c>
       <c r="I16" t="n">
-        <v>-11.39141224111249</v>
+        <v>-11.31818867908856</v>
       </c>
     </row>
     <row r="17">
@@ -951,10 +951,10 @@
         <v>3.829377182780475</v>
       </c>
       <c r="H17" t="n">
-        <v>3.738061587750002e-32</v>
+        <v>1.196172388658729e-31</v>
       </c>
       <c r="I17" t="n">
-        <v>11.80363536367669</v>
+        <v>11.70538346877259</v>
       </c>
     </row>
     <row r="18">
@@ -978,10 +978,10 @@
         <v>0.2868298374685423</v>
       </c>
       <c r="H18" t="n">
-        <v>0.001124132031183372</v>
+        <v>0.0009644551881238153</v>
       </c>
       <c r="I18" t="n">
-        <v>-3.257462265617051</v>
+        <v>-3.300695427568846</v>
       </c>
     </row>
     <row r="19">
@@ -1005,10 +1005,10 @@
         <v>6.689243196656912</v>
       </c>
       <c r="H19" t="n">
-        <v>5.625230911940286e-94</v>
+        <v>8.935120371438574e-93</v>
       </c>
       <c r="I19" t="n">
-        <v>20.56521304421974</v>
+        <v>20.43062486268667</v>
       </c>
     </row>
     <row r="20">
@@ -1032,10 +1032,10 @@
         <v>6.379959272647231</v>
       </c>
       <c r="H20" t="n">
-        <v>9.742353216815597e-105</v>
+        <v>1.481729373107182e-105</v>
       </c>
       <c r="I20" t="n">
-        <v>21.73422033842692</v>
+        <v>21.82051756860907</v>
       </c>
     </row>
     <row r="21">
@@ -1059,10 +1059,10 @@
         <v>5.726266324517253</v>
       </c>
       <c r="H21" t="n">
-        <v>1.166518703885842e-112</v>
+        <v>5.484327550857091e-112</v>
       </c>
       <c r="I21" t="n">
-        <v>22.55622965044033</v>
+        <v>22.4876370959424</v>
       </c>
     </row>
     <row r="22">
@@ -1084,16 +1084,16 @@
         <v>2.860697638597838</v>
       </c>
       <c r="F22" t="n">
-        <v>0.005424722780159436</v>
+        <v>0.005424722780159434</v>
       </c>
       <c r="G22" t="n">
         <v>2.84326149269131</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0005506263901160855</v>
+        <v>0.0005540473458010006</v>
       </c>
       <c r="I22" t="n">
-        <v>3.454836614554206</v>
+        <v>3.453166290299961</v>
       </c>
     </row>
     <row r="23">
@@ -1105,22 +1105,22 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.133503021397445e-26</v>
+        <v>4.133503021397444e-26</v>
       </c>
       <c r="E23" t="n">
         <v>14.4418299974249</v>
       </c>
       <c r="F23" t="n">
-        <v>4.31305663103952e-26</v>
+        <v>4.313056631039521e-26</v>
       </c>
       <c r="G23" t="n">
         <v>14.43272618892365</v>
       </c>
       <c r="H23" t="n">
-        <v>3.063055651416904e-109</v>
+        <v>1.700408807688419e-97</v>
       </c>
       <c r="I23" t="n">
-        <v>22.20514484712804</v>
+        <v>20.9546876391584</v>
       </c>
     </row>
     <row r="24">
@@ -1144,10 +1144,10 @@
         <v>-10.08169399830905</v>
       </c>
       <c r="H24" t="n">
-        <v>1.053394639769707e-55</v>
+        <v>9.909403786726777e-57</v>
       </c>
       <c r="I24" t="n">
-        <v>-15.7229288440841</v>
+        <v>-15.87196205388654</v>
       </c>
     </row>
     <row r="25">
@@ -1171,10 +1171,10 @@
         <v>-6.872079984771239</v>
       </c>
       <c r="H25" t="n">
-        <v>3.253895836922674e-18</v>
+        <v>7.9312294778736e-19</v>
       </c>
       <c r="I25" t="n">
-        <v>-8.70224241593176</v>
+        <v>-8.860982532979264</v>
       </c>
     </row>
     <row r="26">
@@ -1198,10 +1198,10 @@
         <v>-8.158875080482366</v>
       </c>
       <c r="H26" t="n">
-        <v>1.667469705197999e-26</v>
+        <v>1.431882831483472e-28</v>
       </c>
       <c r="I26" t="n">
-        <v>-10.65415786283203</v>
+        <v>-11.08816917839088</v>
       </c>
     </row>
     <row r="27">
@@ -1229,10 +1229,10 @@
         <v>6.483248875259473</v>
       </c>
       <c r="H27" t="n">
-        <v>3.131330043843228e-20</v>
+        <v>4.665513904449939e-20</v>
       </c>
       <c r="I27" t="n">
-        <v>9.214362645026316</v>
+        <v>9.171483989524392</v>
       </c>
     </row>
     <row r="28">
@@ -1256,10 +1256,10 @@
         <v>16.72796635475693</v>
       </c>
       <c r="H28" t="n">
-        <v>8.151957568302565e-155</v>
+        <v>2.58109417204881e-159</v>
       </c>
       <c r="I28" t="n">
-        <v>26.50652111927853</v>
+        <v>26.89400467798536</v>
       </c>
     </row>
     <row r="29">
@@ -1283,10 +1283,10 @@
         <v>-7.25268446927321</v>
       </c>
       <c r="H29" t="n">
-        <v>1.519395650033375e-31</v>
+        <v>4.571296391100679e-31</v>
       </c>
       <c r="I29" t="n">
-        <v>-11.68507825321466</v>
+        <v>-11.59111739818112</v>
       </c>
     </row>
     <row r="30">
@@ -1310,10 +1310,10 @@
         <v>-4.550518363647007</v>
       </c>
       <c r="H30" t="n">
-        <v>1.035603005227789e-12</v>
+        <v>1.15132337411586e-12</v>
       </c>
       <c r="I30" t="n">
-        <v>-7.125690350866612</v>
+        <v>-7.111087232547288</v>
       </c>
     </row>
     <row r="31">
@@ -1337,10 +1337,10 @@
         <v>-3.924371494617405</v>
       </c>
       <c r="H31" t="n">
-        <v>2.31831657476823e-12</v>
+        <v>6.747721159686214e-12</v>
       </c>
       <c r="I31" t="n">
-        <v>-7.013859833549149</v>
+        <v>-6.862898418292664</v>
       </c>
     </row>
     <row r="32">
@@ -1372,10 +1372,10 @@
         <v>-2.053824980528773</v>
       </c>
       <c r="H32" t="n">
-        <v>1.064993660213941e-27</v>
+        <v>1.479426211990881e-26</v>
       </c>
       <c r="I32" t="n">
-        <v>-10.9071883883657</v>
+        <v>-10.66528635668025</v>
       </c>
     </row>
     <row r="33">
@@ -1393,16 +1393,16 @@
         <v>-5.32643073881437</v>
       </c>
       <c r="F33" t="n">
-        <v>4.641747559277946e-07</v>
+        <v>4.641747559277947e-07</v>
       </c>
       <c r="G33" t="n">
         <v>-5.397037255112573</v>
       </c>
       <c r="H33" t="n">
-        <v>5.461023112278413e-60</v>
+        <v>1.333851400561177e-61</v>
       </c>
       <c r="I33" t="n">
-        <v>-16.33613088308612</v>
+        <v>-16.56098822601835</v>
       </c>
     </row>
     <row r="34">
@@ -1426,10 +1426,10 @@
         <v>6.106324913733292</v>
       </c>
       <c r="H34" t="n">
-        <v>4.362329760578391e-13</v>
+        <v>1.439184655900378e-12</v>
       </c>
       <c r="I34" t="n">
-        <v>7.243816055793398</v>
+        <v>7.080227050948953</v>
       </c>
     </row>
     <row r="35">
@@ -1453,10 +1453,10 @@
         <v>4.763429962809396</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01623561232242789</v>
+        <v>0.01894535220142964</v>
       </c>
       <c r="I35" t="n">
-        <v>2.403575538941408</v>
+        <v>2.346604510927215</v>
       </c>
     </row>
     <row r="36">
@@ -1480,10 +1480,10 @@
         <v>4.835883669895765</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0009779537113980925</v>
+        <v>0.001181611798443139</v>
       </c>
       <c r="I36" t="n">
-        <v>3.296793511876819</v>
+        <v>3.243282038831781</v>
       </c>
     </row>
     <row r="37">
@@ -1505,16 +1505,16 @@
         <v>1.283023682049838</v>
       </c>
       <c r="F37" t="n">
-        <v>0.2074807101666616</v>
+        <v>0.2074807101666617</v>
       </c>
       <c r="G37" t="n">
         <v>1.268819249423843</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1640712267021671</v>
+        <v>0.1784363945873845</v>
       </c>
       <c r="I37" t="n">
-        <v>1.391508688809256</v>
+        <v>1.34558499148247</v>
       </c>
     </row>
     <row r="38">
@@ -1538,10 +1538,10 @@
         <v>11.80771920782478</v>
       </c>
       <c r="H38" t="n">
-        <v>3.673254868062138e-72</v>
+        <v>5.158656229513774e-63</v>
       </c>
       <c r="I38" t="n">
-        <v>17.96484153671965</v>
+        <v>16.75554436211863</v>
       </c>
     </row>
     <row r="39">
@@ -1565,10 +1565,10 @@
         <v>-9.991153472191344</v>
       </c>
       <c r="H39" t="n">
-        <v>3.57028761427407e-62</v>
+        <v>8.663344879867317e-48</v>
       </c>
       <c r="I39" t="n">
-        <v>-16.64009876303128</v>
+        <v>-14.5230005383045</v>
       </c>
     </row>
     <row r="40">
@@ -1592,10 +1592,10 @@
         <v>-5.340872939243267</v>
       </c>
       <c r="H40" t="n">
-        <v>5.856346540277147e-20</v>
+        <v>2.663650447286536e-21</v>
       </c>
       <c r="I40" t="n">
-        <v>-9.146950262618788</v>
+        <v>-9.47515496481191</v>
       </c>
     </row>
     <row r="41">
@@ -1619,10 +1619,10 @@
         <v>-5.950148732417835</v>
       </c>
       <c r="H41" t="n">
-        <v>4.197251130367381e-21</v>
+        <v>1.894887519049616e-21</v>
       </c>
       <c r="I41" t="n">
-        <v>-9.427563527204315</v>
+        <v>-9.51064238050604</v>
       </c>
     </row>
     <row r="42">
@@ -1650,10 +1650,10 @@
         <v>2.413154417539551</v>
       </c>
       <c r="H42" t="n">
-        <v>1.52050707900996e-05</v>
+        <v>1.933531764003987e-05</v>
       </c>
       <c r="I42" t="n">
-        <v>4.325696423186593</v>
+        <v>4.272431250462653</v>
       </c>
     </row>
     <row r="43">
@@ -1677,10 +1677,10 @@
         <v>14.82628505412745</v>
       </c>
       <c r="H43" t="n">
-        <v>1.355129894570722e-135</v>
+        <v>1.533034176882243e-126</v>
       </c>
       <c r="I43" t="n">
-        <v>24.78336154946117</v>
+        <v>23.92888865479044</v>
       </c>
     </row>
     <row r="44">
@@ -1704,10 +1704,10 @@
         <v>-12.55196745973415</v>
       </c>
       <c r="H44" t="n">
-        <v>8.841874000289993e-76</v>
+        <v>8.913430203429876e-76</v>
       </c>
       <c r="I44" t="n">
-        <v>-18.42144056370074</v>
+        <v>-18.42100428646772</v>
       </c>
     </row>
     <row r="45">
@@ -1731,10 +1731,10 @@
         <v>-7.147973324123668</v>
       </c>
       <c r="H45" t="n">
-        <v>7.680115822440262e-30</v>
+        <v>2.134815740252233e-26</v>
       </c>
       <c r="I45" t="n">
-        <v>-11.34694293398614</v>
+        <v>-10.63114225812502</v>
       </c>
     </row>
     <row r="46">
@@ -1758,10 +1758,10 @@
         <v>-5.391703759349401</v>
       </c>
       <c r="H46" t="n">
-        <v>1.337709969182684e-16</v>
+        <v>1.518946452831954e-15</v>
       </c>
       <c r="I46" t="n">
-        <v>-8.270167450753494</v>
+        <v>-7.975394672466073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create folder if not existent. remove df_p stuff
</commit_message>
<xml_diff>
--- a/DD_Project/data/Niedermayer/statistical_tests/statistical_tests_results.xlsx
+++ b/DD_Project/data/Niedermayer/statistical_tests/statistical_tests_results.xlsx
@@ -530,10 +530,10 @@
         <v>2.611035721775769</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1005870299094374</v>
+        <v>0.09848601862732026</v>
       </c>
       <c r="I2" t="n">
-        <v>1.642014351456121</v>
+        <v>1.652238118382965</v>
       </c>
     </row>
     <row r="3">
@@ -557,10 +557,10 @@
         <v>-1.886925991587385</v>
       </c>
       <c r="H3" t="n">
-        <v>5.14172098898158e-42</v>
+        <v>1.321290021644665e-41</v>
       </c>
       <c r="I3" t="n">
-        <v>-13.58170251854409</v>
+        <v>-13.51240738922745</v>
       </c>
     </row>
     <row r="4">
@@ -584,10 +584,10 @@
         <v>7.18280400982161</v>
       </c>
       <c r="H4" t="n">
-        <v>2.46192811623977e-69</v>
+        <v>2.039558748889865e-77</v>
       </c>
       <c r="I4" t="n">
-        <v>17.60003022547899</v>
+        <v>18.62434938601493</v>
       </c>
     </row>
     <row r="5">
@@ -611,10 +611,10 @@
         <v>4.604144728265748</v>
       </c>
       <c r="H5" t="n">
-        <v>9.753236417151387e-18</v>
+        <v>2.317154994930742e-17</v>
       </c>
       <c r="I5" t="n">
-        <v>8.576819651182786</v>
+        <v>8.476677804302749</v>
       </c>
     </row>
     <row r="6">
@@ -638,10 +638,10 @@
         <v>4.836262268888744</v>
       </c>
       <c r="H6" t="n">
-        <v>1.070470095212138e-23</v>
+        <v>5.277542374521448e-25</v>
       </c>
       <c r="I6" t="n">
-        <v>10.03491920089278</v>
+        <v>10.32776590728914</v>
       </c>
     </row>
     <row r="7">
@@ -669,10 +669,10 @@
         <v>2.911860544057738</v>
       </c>
       <c r="H7" t="n">
-        <v>0.001396946837793676</v>
+        <v>0.0002792762503104448</v>
       </c>
       <c r="I7" t="n">
-        <v>3.195281150425419</v>
+        <v>3.633801040501866</v>
       </c>
     </row>
     <row r="8">
@@ -696,10 +696,10 @@
         <v>18.26489919888875</v>
       </c>
       <c r="H8" t="n">
-        <v>7.983756059632076e-196</v>
+        <v>2.216290846907834e-174</v>
       </c>
       <c r="I8" t="n">
-        <v>29.85317630367946</v>
+        <v>28.15277166673561</v>
       </c>
     </row>
     <row r="9">
@@ -723,10 +723,10 @@
         <v>-13.95094143674026</v>
       </c>
       <c r="H9" t="n">
-        <v>7.793518645540226e-99</v>
+        <v>3.223078845225822e-97</v>
       </c>
       <c r="I9" t="n">
-        <v>-21.10096151109139</v>
+        <v>-20.92421789370874</v>
       </c>
     </row>
     <row r="10">
@@ -744,16 +744,16 @@
         <v>-8.597604571087324</v>
       </c>
       <c r="F10" t="n">
-        <v>4.090125119497236e-14</v>
+        <v>4.090125119497237e-14</v>
       </c>
       <c r="G10" t="n">
         <v>-8.819416807040355</v>
       </c>
       <c r="H10" t="n">
-        <v>1.626712725324637e-42</v>
+        <v>7.779370280598121e-51</v>
       </c>
       <c r="I10" t="n">
-        <v>-13.66572687144085</v>
+        <v>-14.99615821514027</v>
       </c>
     </row>
     <row r="11">
@@ -777,10 +777,10 @@
         <v>-10.02712355821534</v>
       </c>
       <c r="H11" t="n">
-        <v>3.762217274443967e-48</v>
+        <v>2.148157955288719e-50</v>
       </c>
       <c r="I11" t="n">
-        <v>-14.58005350840661</v>
+        <v>-14.92857245517089</v>
       </c>
     </row>
     <row r="12">
@@ -808,10 +808,10 @@
         <v>6.219060602798643</v>
       </c>
       <c r="H12" t="n">
-        <v>1.283794319129071e-21</v>
+        <v>1.405045832173766e-22</v>
       </c>
       <c r="I12" t="n">
-        <v>9.551057208083092</v>
+        <v>9.777598595581384</v>
       </c>
     </row>
     <row r="13">
@@ -835,10 +835,10 @@
         <v>21.49354292899049</v>
       </c>
       <c r="H13" t="n">
-        <v>1.349055976310105e-250</v>
+        <v>2.330551571583976e-290</v>
       </c>
       <c r="I13" t="n">
-        <v>33.81122331986262</v>
+        <v>36.41653484576065</v>
       </c>
     </row>
     <row r="14">
@@ -862,10 +862,10 @@
         <v>-12.99353752381963</v>
       </c>
       <c r="H14" t="n">
-        <v>1.070148427334821e-102</v>
+        <v>8.225420312876559e-96</v>
       </c>
       <c r="I14" t="n">
-        <v>-21.51739207891101</v>
+        <v>-20.7691777957254</v>
       </c>
     </row>
     <row r="15">
@@ -889,10 +889,10 @@
         <v>-8.073719604570949</v>
       </c>
       <c r="H15" t="n">
-        <v>1.740138330085494e-36</v>
+        <v>8.551553098984214e-38</v>
       </c>
       <c r="I15" t="n">
-        <v>-12.6152458157533</v>
+        <v>-12.8504462250916</v>
       </c>
     </row>
     <row r="16">
@@ -916,10 +916,10 @@
         <v>-6.455361578813921</v>
       </c>
       <c r="H16" t="n">
-        <v>1.0665277478531e-29</v>
+        <v>3.683496002766283e-26</v>
       </c>
       <c r="I16" t="n">
-        <v>-11.31818867908856</v>
+        <v>-10.58015468445819</v>
       </c>
     </row>
     <row r="17">
@@ -951,10 +951,10 @@
         <v>3.829377182780475</v>
       </c>
       <c r="H17" t="n">
-        <v>1.196172388658729e-31</v>
+        <v>1.308917393152356e-31</v>
       </c>
       <c r="I17" t="n">
-        <v>11.70538346877259</v>
+        <v>11.69774092658699</v>
       </c>
     </row>
     <row r="18">
@@ -978,10 +978,10 @@
         <v>0.2868298374685423</v>
       </c>
       <c r="H18" t="n">
-        <v>0.0009644551881238153</v>
+        <v>0.0009446089762037671</v>
       </c>
       <c r="I18" t="n">
-        <v>-3.300695427568846</v>
+        <v>-3.306525069182445</v>
       </c>
     </row>
     <row r="19">
@@ -1005,10 +1005,10 @@
         <v>6.689243196656912</v>
       </c>
       <c r="H19" t="n">
-        <v>8.935120371438574e-93</v>
+        <v>2.45394121593645e-92</v>
       </c>
       <c r="I19" t="n">
-        <v>20.43062486268667</v>
+        <v>20.38123324251259</v>
       </c>
     </row>
     <row r="20">
@@ -1032,10 +1032,10 @@
         <v>6.379959272647231</v>
       </c>
       <c r="H20" t="n">
-        <v>1.481729373107182e-105</v>
+        <v>1.504752556286769e-101</v>
       </c>
       <c r="I20" t="n">
-        <v>21.82051756860907</v>
+        <v>21.39445581604381</v>
       </c>
     </row>
     <row r="21">
@@ -1059,10 +1059,10 @@
         <v>5.726266324517253</v>
       </c>
       <c r="H21" t="n">
-        <v>5.484327550857091e-112</v>
+        <v>1.04114863183972e-112</v>
       </c>
       <c r="I21" t="n">
-        <v>22.4876370959424</v>
+        <v>22.56125994674017</v>
       </c>
     </row>
     <row r="22">
@@ -1084,16 +1084,16 @@
         <v>2.860697638597838</v>
       </c>
       <c r="F22" t="n">
-        <v>0.005424722780159434</v>
+        <v>0.005424722780159436</v>
       </c>
       <c r="G22" t="n">
         <v>2.84326149269131</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0005540473458010006</v>
+        <v>0.0006815864733909085</v>
       </c>
       <c r="I22" t="n">
-        <v>3.453166290299961</v>
+        <v>3.39688081113558</v>
       </c>
     </row>
     <row r="23">
@@ -1105,22 +1105,22 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4.133503021397444e-26</v>
+        <v>4.133503021397445e-26</v>
       </c>
       <c r="E23" t="n">
         <v>14.4418299974249</v>
       </c>
       <c r="F23" t="n">
-        <v>4.313056631039521e-26</v>
+        <v>4.31305663103952e-26</v>
       </c>
       <c r="G23" t="n">
         <v>14.43272618892365</v>
       </c>
       <c r="H23" t="n">
-        <v>1.700408807688419e-97</v>
+        <v>1.281799887524342e-104</v>
       </c>
       <c r="I23" t="n">
-        <v>20.9546876391584</v>
+        <v>21.72161949362362</v>
       </c>
     </row>
     <row r="24">
@@ -1144,10 +1144,10 @@
         <v>-10.08169399830905</v>
       </c>
       <c r="H24" t="n">
-        <v>9.909403786726777e-57</v>
+        <v>3.341975839169662e-54</v>
       </c>
       <c r="I24" t="n">
-        <v>-15.87196205388654</v>
+        <v>-15.50239518950835</v>
       </c>
     </row>
     <row r="25">
@@ -1171,10 +1171,10 @@
         <v>-6.872079984771239</v>
       </c>
       <c r="H25" t="n">
-        <v>7.9312294778736e-19</v>
+        <v>1.344667035640849e-19</v>
       </c>
       <c r="I25" t="n">
-        <v>-8.860982532979264</v>
+        <v>-9.056691940797204</v>
       </c>
     </row>
     <row r="26">
@@ -1198,10 +1198,10 @@
         <v>-8.158875080482366</v>
       </c>
       <c r="H26" t="n">
-        <v>1.431882831483472e-28</v>
+        <v>6.560262656697334e-28</v>
       </c>
       <c r="I26" t="n">
-        <v>-11.08816917839088</v>
+        <v>-10.95115920964167</v>
       </c>
     </row>
     <row r="27">
@@ -1229,10 +1229,10 @@
         <v>6.483248875259473</v>
       </c>
       <c r="H27" t="n">
-        <v>4.665513904449939e-20</v>
+        <v>2.169412589807753e-20</v>
       </c>
       <c r="I27" t="n">
-        <v>9.171483989524392</v>
+        <v>9.253656569601779</v>
       </c>
     </row>
     <row r="28">
@@ -1256,10 +1256,10 @@
         <v>16.72796635475693</v>
       </c>
       <c r="H28" t="n">
-        <v>2.58109417204881e-159</v>
+        <v>1.071242209843778e-158</v>
       </c>
       <c r="I28" t="n">
-        <v>26.89400467798536</v>
+        <v>26.84110715351077</v>
       </c>
     </row>
     <row r="29">
@@ -1283,10 +1283,10 @@
         <v>-7.25268446927321</v>
       </c>
       <c r="H29" t="n">
-        <v>4.571296391100679e-31</v>
+        <v>3.66317047257038e-32</v>
       </c>
       <c r="I29" t="n">
-        <v>-11.59111739818112</v>
+        <v>-11.80533776269232</v>
       </c>
     </row>
     <row r="30">
@@ -1310,10 +1310,10 @@
         <v>-4.550518363647007</v>
       </c>
       <c r="H30" t="n">
-        <v>1.15132337411586e-12</v>
+        <v>1.388731868567314e-12</v>
       </c>
       <c r="I30" t="n">
-        <v>-7.111087232547288</v>
+        <v>-7.08517052951575</v>
       </c>
     </row>
     <row r="31">
@@ -1337,10 +1337,10 @@
         <v>-3.924371494617405</v>
       </c>
       <c r="H31" t="n">
-        <v>6.747721159686214e-12</v>
+        <v>1.502438606793471e-11</v>
       </c>
       <c r="I31" t="n">
-        <v>-6.862898418292664</v>
+        <v>-6.747664496003302</v>
       </c>
     </row>
     <row r="32">
@@ -1372,10 +1372,10 @@
         <v>-2.053824980528773</v>
       </c>
       <c r="H32" t="n">
-        <v>1.479426211990881e-26</v>
+        <v>2.894783167268939e-27</v>
       </c>
       <c r="I32" t="n">
-        <v>-10.66528635668025</v>
+        <v>-10.81588711661282</v>
       </c>
     </row>
     <row r="33">
@@ -1393,16 +1393,16 @@
         <v>-5.32643073881437</v>
       </c>
       <c r="F33" t="n">
-        <v>4.641747559277947e-07</v>
+        <v>4.641747559277946e-07</v>
       </c>
       <c r="G33" t="n">
         <v>-5.397037255112573</v>
       </c>
       <c r="H33" t="n">
-        <v>1.333851400561177e-61</v>
+        <v>5.176275505456987e-59</v>
       </c>
       <c r="I33" t="n">
-        <v>-16.56098822601835</v>
+        <v>-16.19839225683151</v>
       </c>
     </row>
     <row r="34">
@@ -1426,10 +1426,10 @@
         <v>6.106324913733292</v>
       </c>
       <c r="H34" t="n">
-        <v>1.439184655900378e-12</v>
+        <v>3.838287071939599e-12</v>
       </c>
       <c r="I34" t="n">
-        <v>7.080227050948953</v>
+        <v>6.943011299358002</v>
       </c>
     </row>
     <row r="35">
@@ -1453,10 +1453,10 @@
         <v>4.763429962809396</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01894535220142964</v>
+        <v>0.0176184553557072</v>
       </c>
       <c r="I35" t="n">
-        <v>2.346604510927215</v>
+        <v>2.37354061303342</v>
       </c>
     </row>
     <row r="36">
@@ -1480,10 +1480,10 @@
         <v>4.835883669895765</v>
       </c>
       <c r="H36" t="n">
-        <v>0.001181611798443139</v>
+        <v>0.0008382126776864868</v>
       </c>
       <c r="I36" t="n">
-        <v>3.243282038831781</v>
+        <v>3.339857898741211</v>
       </c>
     </row>
     <row r="37">
@@ -1505,16 +1505,16 @@
         <v>1.283023682049838</v>
       </c>
       <c r="F37" t="n">
-        <v>0.2074807101666617</v>
+        <v>0.2074807101666616</v>
       </c>
       <c r="G37" t="n">
         <v>1.268819249423843</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1784363945873845</v>
+        <v>0.1899958221220994</v>
       </c>
       <c r="I37" t="n">
-        <v>1.34558499148247</v>
+        <v>1.310591471503704</v>
       </c>
     </row>
     <row r="38">
@@ -1538,10 +1538,10 @@
         <v>11.80771920782478</v>
       </c>
       <c r="H38" t="n">
-        <v>5.158656229513774e-63</v>
+        <v>4.176791926354502e-59</v>
       </c>
       <c r="I38" t="n">
-        <v>16.75554436211863</v>
+        <v>16.21158168338971</v>
       </c>
     </row>
     <row r="39">
@@ -1565,10 +1565,10 @@
         <v>-9.991153472191344</v>
       </c>
       <c r="H39" t="n">
-        <v>8.663344879867317e-48</v>
+        <v>7.045463199321931e-43</v>
       </c>
       <c r="I39" t="n">
-        <v>-14.5230005383045</v>
+        <v>-13.72650113197182</v>
       </c>
     </row>
     <row r="40">
@@ -1592,10 +1592,10 @@
         <v>-5.340872939243267</v>
       </c>
       <c r="H40" t="n">
-        <v>2.663650447286536e-21</v>
+        <v>5.983863907945237e-21</v>
       </c>
       <c r="I40" t="n">
-        <v>-9.47515496481191</v>
+        <v>-9.39028409075843</v>
       </c>
     </row>
     <row r="41">
@@ -1619,10 +1619,10 @@
         <v>-5.950148732417835</v>
       </c>
       <c r="H41" t="n">
-        <v>1.894887519049616e-21</v>
+        <v>1.348493453021991e-22</v>
       </c>
       <c r="I41" t="n">
-        <v>-9.51064238050604</v>
+        <v>-9.781756727778122</v>
       </c>
     </row>
     <row r="42">
@@ -1650,10 +1650,10 @@
         <v>2.413154417539551</v>
       </c>
       <c r="H42" t="n">
-        <v>1.933531764003987e-05</v>
+        <v>1.668480096421356e-05</v>
       </c>
       <c r="I42" t="n">
-        <v>4.272431250462653</v>
+        <v>4.30518265926056</v>
       </c>
     </row>
     <row r="43">
@@ -1677,10 +1677,10 @@
         <v>14.82628505412745</v>
       </c>
       <c r="H43" t="n">
-        <v>1.533034176882243e-126</v>
+        <v>1.125374071928214e-124</v>
       </c>
       <c r="I43" t="n">
-        <v>23.92888865479044</v>
+        <v>23.74899321397551</v>
       </c>
     </row>
     <row r="44">
@@ -1704,10 +1704,10 @@
         <v>-12.55196745973415</v>
       </c>
       <c r="H44" t="n">
-        <v>8.913430203429876e-76</v>
+        <v>4.415798392557715e-82</v>
       </c>
       <c r="I44" t="n">
-        <v>-18.42100428646772</v>
+        <v>-19.19082428022793</v>
       </c>
     </row>
     <row r="45">
@@ -1731,10 +1731,10 @@
         <v>-7.147973324123668</v>
       </c>
       <c r="H45" t="n">
-        <v>2.134815740252233e-26</v>
+        <v>1.70807036917321e-28</v>
       </c>
       <c r="I45" t="n">
-        <v>-10.63114225812502</v>
+        <v>-11.07237794302584</v>
       </c>
     </row>
     <row r="46">
@@ -1758,10 +1758,10 @@
         <v>-5.391703759349401</v>
       </c>
       <c r="H46" t="n">
-        <v>1.518946452831954e-15</v>
+        <v>6.831209819502281e-17</v>
       </c>
       <c r="I46" t="n">
-        <v>-7.975394672466073</v>
+        <v>-8.34991502017291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>